<commit_message>
years as fixed variable
</commit_message>
<xml_diff>
--- a/input_estimates.xlsx
+++ b/input_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9af5f397540487a4/R/Nuts_and_chicken/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="11_AD4DB114E441178AC67DF459BED3DF1C693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1624EF2-DA36-4CE8-BA4D-ABEBE6978FF7}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="11_AD4DB114E441178AC67DF459BED3DF1C693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{512A0395-FD75-4BE3-91C1-536AE0F55B2D}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="-12390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="81">
   <si>
     <t>variable</t>
   </si>
@@ -162,12 +162,6 @@
     <t>€/m^3</t>
   </si>
   <si>
-    <t>dt</t>
-  </si>
-  <si>
-    <t>€/dt</t>
-  </si>
-  <si>
     <t>Cost for getting protective animals</t>
   </si>
   <si>
@@ -259,6 +253,21 @@
   </si>
   <si>
     <t>€/h</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>0.34</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>€/t</t>
   </si>
 </sst>
 </file>
@@ -332,12 +341,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -618,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,8 +670,14 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B2" s="5">
+        <v>200</v>
+      </c>
       <c r="C2" t="s">
         <v>35</v>
+      </c>
+      <c r="D2" s="5">
+        <v>500</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
@@ -675,9 +693,15 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="5">
+        <v>400</v>
+      </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
+      <c r="D3" s="5">
+        <v>600</v>
+      </c>
       <c r="E3" t="s">
         <v>36</v>
       </c>
@@ -685,21 +709,21 @@
         <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>5</v>
+      <c r="B4" s="5">
+        <v>1500</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
       </c>
-      <c r="D4">
-        <v>14</v>
+      <c r="D4" s="5">
+        <v>5000</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
@@ -708,16 +732,22 @@
         <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B5" s="5">
+        <v>500</v>
+      </c>
       <c r="C5" t="s">
         <v>35</v>
       </c>
+      <c r="D5" s="5">
+        <v>1500</v>
+      </c>
       <c r="E5" t="s">
         <v>36</v>
       </c>
@@ -725,16 +755,22 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="5">
+        <v>1500</v>
+      </c>
       <c r="C6" t="s">
         <v>35</v>
       </c>
+      <c r="D6" s="5">
+        <v>4000</v>
+      </c>
       <c r="E6" t="s">
         <v>36</v>
       </c>
@@ -742,16 +778,22 @@
         <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B7" s="5">
+        <v>150</v>
+      </c>
       <c r="C7" t="s">
         <v>35</v>
       </c>
+      <c r="D7" s="5">
+        <v>500</v>
+      </c>
       <c r="E7" t="s">
         <v>36</v>
       </c>
@@ -759,16 +801,22 @@
         <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B8" s="5">
+        <v>5000</v>
+      </c>
       <c r="C8" t="s">
         <v>35</v>
       </c>
+      <c r="D8" s="5">
+        <v>15000</v>
+      </c>
       <c r="E8" t="s">
         <v>36</v>
       </c>
@@ -776,16 +824,22 @@
         <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B9" s="5">
+        <v>150</v>
+      </c>
       <c r="C9" t="s">
         <v>35</v>
       </c>
+      <c r="D9" s="5">
+        <v>250</v>
+      </c>
       <c r="E9" t="s">
         <v>36</v>
       </c>
@@ -793,16 +847,22 @@
         <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B10" s="5">
+        <v>50</v>
+      </c>
       <c r="C10" t="s">
         <v>35</v>
       </c>
+      <c r="D10" s="5">
+        <v>100</v>
+      </c>
       <c r="E10" t="s">
         <v>36</v>
       </c>
@@ -810,16 +870,22 @@
         <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B11" s="5">
+        <v>100</v>
+      </c>
       <c r="C11" t="s">
         <v>35</v>
       </c>
+      <c r="D11" s="5">
+        <v>200</v>
+      </c>
       <c r="E11" t="s">
         <v>36</v>
       </c>
@@ -827,16 +893,22 @@
         <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B12" s="5">
+        <v>5</v>
+      </c>
       <c r="C12" t="s">
         <v>35</v>
       </c>
+      <c r="D12" s="5">
+        <v>15</v>
+      </c>
       <c r="E12" t="s">
         <v>36</v>
       </c>
@@ -844,16 +916,22 @@
         <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B13" s="5">
+        <v>20</v>
+      </c>
       <c r="C13" t="s">
         <v>35</v>
       </c>
+      <c r="D13" s="5">
+        <v>30</v>
+      </c>
       <c r="E13" t="s">
         <v>36</v>
       </c>
@@ -861,16 +939,22 @@
         <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B14" s="5">
+        <v>5</v>
+      </c>
       <c r="C14" t="s">
         <v>35</v>
       </c>
+      <c r="D14" s="5">
+        <v>10</v>
+      </c>
       <c r="E14" t="s">
         <v>36</v>
       </c>
@@ -878,16 +962,22 @@
         <v>38</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B15" s="5">
+        <v>500</v>
+      </c>
       <c r="C15" t="s">
         <v>35</v>
       </c>
+      <c r="D15" s="5">
+        <v>1000</v>
+      </c>
       <c r="E15" t="s">
         <v>36</v>
       </c>
@@ -895,16 +985,22 @@
         <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B16" s="5">
+        <v>200</v>
+      </c>
       <c r="C16" t="s">
         <v>35</v>
       </c>
+      <c r="D16" s="5">
+        <v>500</v>
+      </c>
       <c r="E16" t="s">
         <v>36</v>
       </c>
@@ -912,16 +1008,22 @@
         <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="B17" s="5">
+        <v>100</v>
+      </c>
       <c r="C17" t="s">
         <v>35</v>
       </c>
+      <c r="D17" s="5">
+        <v>300</v>
+      </c>
       <c r="E17" t="s">
         <v>36</v>
       </c>
@@ -929,50 +1031,68 @@
         <v>38</v>
       </c>
       <c r="G17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
       </c>
+      <c r="D18" s="5">
+        <v>1</v>
+      </c>
       <c r="E18" t="s">
         <v>36</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="B19" s="5">
+        <v>2000</v>
+      </c>
       <c r="C19" t="s">
         <v>35</v>
       </c>
+      <c r="D19" s="5">
+        <v>5000</v>
+      </c>
       <c r="E19" t="s">
         <v>36</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B20" s="5">
+        <v>200</v>
+      </c>
       <c r="C20" t="s">
         <v>35</v>
       </c>
+      <c r="D20" s="5">
+        <v>650</v>
+      </c>
       <c r="E20" t="s">
         <v>36</v>
       </c>
@@ -980,15 +1100,21 @@
         <v>38</v>
       </c>
       <c r="G20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="B21" s="5">
+        <v>20</v>
+      </c>
       <c r="C21" t="s">
         <v>35</v>
+      </c>
+      <c r="D21" s="5">
+        <v>100</v>
       </c>
       <c r="E21" t="s">
         <v>36</v>
@@ -997,15 +1123,21 @@
         <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="B22" s="5">
+        <v>200</v>
+      </c>
       <c r="C22" t="s">
         <v>35</v>
+      </c>
+      <c r="D22" s="5">
+        <v>400</v>
       </c>
       <c r="E22" t="s">
         <v>36</v>
@@ -1014,15 +1146,21 @@
         <v>39</v>
       </c>
       <c r="G22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="B23" s="5">
+        <v>100</v>
+      </c>
       <c r="C23" t="s">
         <v>35</v>
+      </c>
+      <c r="D23" s="5">
+        <v>700</v>
       </c>
       <c r="E23" t="s">
         <v>36</v>
@@ -1031,15 +1169,21 @@
         <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B24" s="5">
+        <v>12</v>
+      </c>
       <c r="C24" t="s">
         <v>35</v>
+      </c>
+      <c r="D24" s="5">
+        <v>20</v>
       </c>
       <c r="E24" t="s">
         <v>36</v>
@@ -1048,15 +1192,21 @@
         <v>39</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="B25" s="5">
+        <v>55000</v>
+      </c>
       <c r="C25" t="s">
         <v>35</v>
+      </c>
+      <c r="D25" s="5">
+        <v>130000</v>
       </c>
       <c r="E25" t="s">
         <v>36</v>
@@ -1065,15 +1215,21 @@
         <v>42</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="B26" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="C26" t="s">
         <v>35</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="E26" t="s">
         <v>36</v>
@@ -1082,15 +1238,21 @@
         <v>40</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="B27" s="5">
+        <v>500</v>
+      </c>
       <c r="C27" t="s">
         <v>35</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1000</v>
       </c>
       <c r="E27" t="s">
         <v>36</v>
@@ -1099,15 +1261,21 @@
         <v>43</v>
       </c>
       <c r="G27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
       <c r="C28" t="s">
         <v>35</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2</v>
       </c>
       <c r="E28" t="s">
         <v>36</v>
@@ -1116,42 +1284,57 @@
         <v>44</v>
       </c>
       <c r="G28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="B29" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="C29" t="s">
         <v>35</v>
       </c>
+      <c r="D29" s="5">
+        <v>1</v>
+      </c>
       <c r="E29" t="s">
         <v>36</v>
       </c>
       <c r="F29" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="B30" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="C30" t="s">
         <v>35</v>
       </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
       <c r="E30" t="s">
         <v>36</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed tree maintaining and harvest to the working hour system
</commit_message>
<xml_diff>
--- a/input_estimates.xlsx
+++ b/input_estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a631459e6cf3f3cb/Uni/Master/2021_ss_decision-analysis/Agroforestry/Nuts_and_chicken/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="341" documentId="8_{3568966E-F10A-4A87-8770-2C8F7733F410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDE5501F-8ED8-4340-B416-730D4A662865}"/>
+  <xr:revisionPtr revIDLastSave="351" documentId="8_{3568966E-F10A-4A87-8770-2C8F7733F410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DAEEB8B-6D1D-4655-B61E-C5E808FA507D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{374AAA1E-B073-4CF1-B979-99CE47E0D28D}"/>
   </bookViews>
@@ -319,18 +319,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -345,12 +339,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -667,13 +660,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B142AC-1DE2-46C2-BBE5-78F1603E233D}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="37.77734375" customWidth="1"/>
     <col min="6" max="6" width="39" customWidth="1"/>
     <col min="7" max="7" width="50.109375" customWidth="1"/>
   </cols>
@@ -816,23 +809,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>35</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1">
         <v>60</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -856,23 +849,23 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="4">
-        <v>400</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4">
-        <v>600</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="B9" s="1">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -881,13 +874,13 @@
         <v>19</v>
       </c>
       <c r="B10" s="1">
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1">
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
@@ -1110,13 +1103,13 @@
         <v>30</v>
       </c>
       <c r="B21" s="1">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="1">
-        <v>4500</v>
+        <v>4000</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>9</v>
@@ -1174,23 +1167,23 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="1">
         <v>12</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1">
         <v>20</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="4" t="s">
+      <c r="E24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added text to markdown and added co2 emitter eggs
</commit_message>
<xml_diff>
--- a/input_estimates.xlsx
+++ b/input_estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive\Uni\Master\2021_ss_decision-analysis\Agroforestry\Nuts_and_chicken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792394C3-B44C-4BD6-8F59-60B5BFA5CB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02802EA5-09E9-4F89-BAC0-3BD9727703CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{374AAA1E-B073-4CF1-B979-99CE47E0D28D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="165">
   <si>
     <t>variable</t>
   </si>
@@ -523,6 +523,12 @@
   </si>
   <si>
     <t>Summerbarley price</t>
+  </si>
+  <si>
+    <t>co2_per_egg</t>
+  </si>
+  <si>
+    <t>CO2 per Egg</t>
   </si>
 </sst>
 </file>
@@ -928,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B142AC-1DE2-46C2-BBE5-78F1603E233D}">
-  <dimension ref="A1:H86"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2415,323 +2421,343 @@
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B71" s="11">
-        <v>2.5</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="11">
-        <v>3.5</v>
-      </c>
-      <c r="E71" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="11" t="s">
-        <v>132</v>
+    <row r="71" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B71" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="9">
+        <v>0.16</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B72" s="11">
-        <v>350</v>
+        <v>2.5</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D72" s="11">
-        <v>500</v>
+        <v>3.5</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B73" s="11">
-        <v>4</v>
+        <v>350</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D73" s="11">
-        <v>5.5</v>
+        <v>500</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B74" s="11">
-        <v>140</v>
+        <v>4</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D74" s="11">
-        <v>200</v>
+        <v>5.5</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B75" s="11">
-        <v>1.5</v>
+        <v>140</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D75" s="11">
-        <v>2.5</v>
+        <v>200</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B76" s="11">
-        <v>320</v>
+        <v>1.5</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D76" s="11">
-        <v>400</v>
+        <v>2.5</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B77" s="11">
-        <v>4</v>
+        <v>320</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="11">
-        <v>5.5</v>
+        <v>400</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B78" s="11">
-        <v>120</v>
+        <v>4</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D78" s="11">
-        <v>160</v>
+        <v>5.5</v>
       </c>
       <c r="E78" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B79" s="11">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D79" s="11">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B80" s="11">
-        <v>400</v>
+        <v>2</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D80" s="11">
-        <v>500</v>
+        <v>4</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B81" s="11">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D81" s="11">
-        <v>6</v>
+        <v>500</v>
       </c>
       <c r="E81" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B82" s="11">
-        <v>130</v>
+        <v>4</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D82" s="11">
-        <v>170</v>
+        <v>6</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B83" s="11">
-        <v>1.5</v>
+        <v>130</v>
       </c>
       <c r="C83" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D83" s="11">
-        <v>2.5</v>
+        <v>170</v>
       </c>
       <c r="E83" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B84" s="11">
-        <v>300</v>
+        <v>1.5</v>
       </c>
       <c r="C84" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D84" s="11">
-        <v>400</v>
+        <v>2.5</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B85" s="11">
-        <v>3.5</v>
+        <v>300</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D85" s="11">
-        <v>5.5</v>
+        <v>400</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B86" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B86" s="11">
+      <c r="B87" s="11">
         <v>150</v>
       </c>
-      <c r="C86" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D86" s="11">
+      <c r="C87" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="11">
         <v>210</v>
       </c>
-      <c r="E86" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="11" t="s">
+      <c r="E87" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="11" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed chickens so that 50 or 200 chickens can be chosen. 200 weirdly is now more profitable than the 200 from the version before... I dont know why
</commit_message>
<xml_diff>
--- a/input_estimates.xlsx
+++ b/input_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive\Uni\Master\2021_ss_decision-analysis\Agroforestry\Nuts_and_chicken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02802EA5-09E9-4F89-BAC0-3BD9727703CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97621374-8F84-4E45-921A-4444742D7244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{374AAA1E-B073-4CF1-B979-99CE47E0D28D}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{374AAA1E-B073-4CF1-B979-99CE47E0D28D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="166">
   <si>
     <t>variable</t>
   </si>
@@ -318,30 +318,12 @@
     <t>truffle_harvest_costs</t>
   </si>
   <si>
-    <t>number_of_chicken</t>
-  </si>
-  <si>
     <t>chicken_replacement_cost</t>
   </si>
   <si>
-    <t>initial_chicken_mobile_cost</t>
-  </si>
-  <si>
-    <t>maintaining_chicken_mobile</t>
-  </si>
-  <si>
-    <t>chicken_feed</t>
-  </si>
-  <si>
     <t>feed_cost</t>
   </si>
   <si>
-    <t>working_hours_chicken</t>
-  </si>
-  <si>
-    <t>eggs</t>
-  </si>
-  <si>
     <t>eggs_price</t>
   </si>
   <si>
@@ -351,9 +333,6 @@
     <t>Truffle harvest cost</t>
   </si>
   <si>
-    <t>Number of chicken</t>
-  </si>
-  <si>
     <t>Price per chicken</t>
   </si>
   <si>
@@ -369,18 +348,12 @@
     <t>Price eggs</t>
   </si>
   <si>
-    <t>Feed in kg</t>
-  </si>
-  <si>
     <t>maintaining_trees_h_3</t>
   </si>
   <si>
     <t>Working hours chicken</t>
   </si>
   <si>
-    <t>Eggs per year</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -529,6 +502,36 @@
   </si>
   <si>
     <t>CO2 per Egg</t>
+  </si>
+  <si>
+    <t>egg_per_hen</t>
+  </si>
+  <si>
+    <t>Eggs per Hen</t>
+  </si>
+  <si>
+    <t>feed_per_hen</t>
+  </si>
+  <si>
+    <t>working_hours_chicken_1</t>
+  </si>
+  <si>
+    <t>maintaining_chicken_mobile_1</t>
+  </si>
+  <si>
+    <t>initial_chicken_mobile_cost_1</t>
+  </si>
+  <si>
+    <t>Feed per Hen</t>
+  </si>
+  <si>
+    <t>initial_chicken_mobile_cost_2</t>
+  </si>
+  <si>
+    <t>maintaining_chicken_mobile_2</t>
+  </si>
+  <si>
+    <t>working_hours_chicken_2</t>
   </si>
 </sst>
 </file>
@@ -934,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B142AC-1DE2-46C2-BBE5-78F1603E233D}">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1208,12 +1211,14 @@
     </row>
     <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B13" s="1">
         <v>16</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D13" s="1">
         <v>25</v>
       </c>
@@ -1230,13 +1235,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>9</v>
@@ -1374,7 +1379,7 @@
     </row>
     <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B21" s="1">
         <v>2700</v>
@@ -1395,7 +1400,7 @@
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B22" s="1">
         <v>7000</v>
@@ -1955,7 +1960,7 @@
         <v>44</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1978,12 +1983,12 @@
         <v>47</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B50" s="2">
         <v>5</v>
@@ -2001,7 +2006,7 @@
         <v>50</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2024,7 +2029,7 @@
         <v>55</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2047,7 +2052,7 @@
         <v>90</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2067,10 +2072,10 @@
         <v>9</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2090,10 +2095,10 @@
         <v>9</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2113,15 +2118,15 @@
         <v>9</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B56" s="2">
         <v>400</v>
@@ -2142,7 +2147,7 @@
     </row>
     <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B57" s="2">
         <v>40</v>
@@ -2166,599 +2171,639 @@
         <v>94</v>
       </c>
       <c r="B58" s="8">
-        <v>225</v>
+        <v>7</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D58" s="8">
-        <v>225</v>
+        <v>13</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="B59" s="8">
-        <v>9</v>
+        <v>30000</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D59" s="8">
-        <v>13</v>
+        <v>40000</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
       <c r="B60" s="8">
-        <v>30000</v>
+        <v>500</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="8">
-        <v>40000</v>
+        <v>1500</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B61" s="8">
-        <v>1000</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="8">
-        <v>1500</v>
+        <v>0.34</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>98</v>
+        <v>159</v>
       </c>
       <c r="B62" s="8">
-        <v>7000</v>
+        <v>250</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D62" s="8">
-        <v>8000</v>
+        <v>360</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="B63" s="8">
-        <v>0.28000000000000003</v>
+        <v>290</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D63" s="8">
-        <v>0.34</v>
+        <v>310</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="B64" s="8">
-        <v>250</v>
+        <v>30</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D64" s="8">
-        <v>360</v>
+        <v>40</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="B65" s="8">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D65" s="8">
-        <v>55000</v>
+        <v>8000</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="B66" s="8">
+        <v>100</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="8">
+        <v>500</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B67" s="8">
+        <v>60</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="8">
+        <v>90</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="8">
         <v>0.25</v>
       </c>
-      <c r="C66" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="8">
+      <c r="C68" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="8">
         <v>0.3</v>
       </c>
-      <c r="E66" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B67" s="9">
-        <v>1000</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="9">
-        <v>1000</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B68" s="9">
-        <v>6</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="9">
-        <v>12</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>128</v>
+      <c r="E68" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B69" s="9">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D69" s="9">
-        <v>7</v>
+        <v>1000</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B70" s="9">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D70" s="9">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="E70" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="B71" s="9">
+        <v>3</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="9">
+        <v>7</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" s="9">
+        <v>45</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="9">
+        <v>70</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B73" s="9">
         <v>0.1</v>
       </c>
-      <c r="C71" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="9">
+      <c r="C73" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="9">
         <v>0.16</v>
       </c>
-      <c r="E71" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B72" s="11">
-        <v>2.5</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="11">
-        <v>3.5</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B73" s="11">
-        <v>350</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="11">
-        <v>500</v>
-      </c>
-      <c r="E73" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="11" t="s">
-        <v>134</v>
+      <c r="E73" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="B74" s="11">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D74" s="11">
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B75" s="11">
-        <v>140</v>
+        <v>350</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D75" s="11">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B76" s="11">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D76" s="11">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B77" s="11">
-        <v>320</v>
+        <v>140</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="11">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B78" s="11">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D78" s="11">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="E78" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B79" s="11">
-        <v>120</v>
+        <v>320</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D79" s="11">
-        <v>160</v>
+        <v>400</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B80" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D80" s="11">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B81" s="11">
-        <v>400</v>
+        <v>120</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D81" s="11">
-        <v>500</v>
+        <v>160</v>
       </c>
       <c r="E81" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B82" s="11">
+        <v>2</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="11">
         <v>4</v>
       </c>
-      <c r="C82" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D82" s="11">
-        <v>6</v>
-      </c>
       <c r="E82" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B83" s="11">
-        <v>130</v>
+        <v>400</v>
       </c>
       <c r="C83" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D83" s="11">
-        <v>170</v>
+        <v>500</v>
       </c>
       <c r="E83" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B84" s="11">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C84" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D84" s="11">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B85" s="11">
-        <v>300</v>
+        <v>130</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D85" s="11">
-        <v>400</v>
+        <v>170</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B86" s="11">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="C86" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D86" s="11">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B87" s="11">
+        <v>300</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="11">
+        <v>400</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="C87" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87" s="11">
+      <c r="B88" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B89" s="11">
+        <v>150</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="11">
         <v>210</v>
       </c>
-      <c r="E87" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F87" s="11" t="s">
-        <v>162</v>
+      <c r="E89" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added soc increase due to landscape change to co2 certificates
</commit_message>
<xml_diff>
--- a/input_estimates.xlsx
+++ b/input_estimates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive\Uni\Master\2021_ss_decision-analysis\Agroforestry\Nuts_and_chicken\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a631459e6cf3f3cb/Uni/Master/2021_ss_decision-analysis/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97621374-8F84-4E45-921A-4444742D7244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{97621374-8F84-4E45-921A-4444742D7244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{601B31E5-8088-4AB9-90EA-578960E3BFD7}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{374AAA1E-B073-4CF1-B979-99CE47E0D28D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="172">
   <si>
     <t>variable</t>
   </si>
@@ -532,6 +532,24 @@
   </si>
   <si>
     <t>working_hours_chicken_2</t>
+  </si>
+  <si>
+    <t>soil_stones</t>
+  </si>
+  <si>
+    <t>Part of stones in soil in %</t>
+  </si>
+  <si>
+    <t>landuse_increase_soc</t>
+  </si>
+  <si>
+    <t>soc</t>
+  </si>
+  <si>
+    <t>SOC in area of interest in kg</t>
+  </si>
+  <si>
+    <t>SOC increase</t>
   </si>
 </sst>
 </file>
@@ -937,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B142AC-1DE2-46C2-BBE5-78F1603E233D}">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2468,341 +2486,401 @@
     </row>
     <row r="73" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B73" s="9">
+        <v>0.35</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B74" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B75" s="9">
+        <v>33000</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="9">
+        <v>41000</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B73" s="9">
+      <c r="B76" s="9">
         <v>0.1</v>
       </c>
-      <c r="C73" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="9">
+      <c r="C76" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="9">
         <v>0.16</v>
       </c>
-      <c r="E73" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="9" t="s">
+      <c r="E76" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="9" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B74" s="11">
-        <v>2.5</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="11">
-        <v>3.5</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B75" s="11">
-        <v>350</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="11">
-        <v>500</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B76" s="11">
-        <v>4</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="11">
-        <v>5.5</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B77" s="11">
-        <v>140</v>
+        <v>2.5</v>
       </c>
       <c r="C77" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="11">
-        <v>200</v>
+        <v>3.5</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B78" s="11">
-        <v>1.5</v>
+        <v>350</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D78" s="11">
-        <v>2.5</v>
+        <v>500</v>
       </c>
       <c r="E78" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B79" s="11">
-        <v>320</v>
+        <v>4</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D79" s="11">
-        <v>400</v>
+        <v>5.5</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B80" s="11">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D80" s="11">
-        <v>5.5</v>
+        <v>200</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B81" s="11">
-        <v>120</v>
+        <v>1.5</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D81" s="11">
-        <v>160</v>
+        <v>2.5</v>
       </c>
       <c r="E81" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B82" s="11">
-        <v>2</v>
+        <v>320</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D82" s="11">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B83" s="11">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="C83" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D83" s="11">
-        <v>500</v>
+        <v>5.5</v>
       </c>
       <c r="E83" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B84" s="11">
-        <v>4</v>
+        <v>120</v>
       </c>
       <c r="C84" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D84" s="11">
-        <v>6</v>
+        <v>160</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B85" s="11">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D85" s="11">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B86" s="11">
-        <v>1.5</v>
+        <v>400</v>
       </c>
       <c r="C86" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D86" s="11">
-        <v>2.5</v>
+        <v>500</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B87" s="11">
-        <v>300</v>
+        <v>4</v>
       </c>
       <c r="C87" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D87" s="11">
-        <v>400</v>
+        <v>6</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B88" s="11">
-        <v>3.5</v>
+        <v>130</v>
       </c>
       <c r="C88" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D88" s="11">
-        <v>5.5</v>
+        <v>170</v>
       </c>
       <c r="E88" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F88" s="11" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B89" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B90" s="11">
+        <v>300</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" s="11">
+        <v>400</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B91" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B89" s="11">
+      <c r="B92" s="11">
         <v>150</v>
       </c>
-      <c r="C89" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89" s="11">
+      <c r="C92" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="11">
         <v>210</v>
       </c>
-      <c r="E89" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F89" s="11" t="s">
+      <c r="E92" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="11" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed list of sources
</commit_message>
<xml_diff>
--- a/input_estimates.xlsx
+++ b/input_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a631459e6cf3f3cb/Uni/Master/2021_ss_decision-analysis/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{97621374-8F84-4E45-921A-4444742D7244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A965EADF-137E-446C-9195-A1DBCB074138}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{97621374-8F84-4E45-921A-4444742D7244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A355593-97C5-422F-9FF0-EDD978DFF8C0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{374AAA1E-B073-4CF1-B979-99CE47E0D28D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{374AAA1E-B073-4CF1-B979-99CE47E0D28D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="202">
   <si>
     <t>variable</t>
   </si>
@@ -550,13 +550,103 @@
   </si>
   <si>
     <t>SOC increase</t>
+  </si>
+  <si>
+    <t>https://daten.ktbl.de/dslkrpflanze/postHv.html#Ergebnis</t>
+  </si>
+  <si>
+    <t>http://www.haselnussanbau-verein.de/index.html</t>
+  </si>
+  <si>
+    <t>http://www.haselnussanbau-verein.de/index.html - and multiple references in online shops</t>
+  </si>
+  <si>
+    <t>https://www.dwd.de/DE/wetter/wetterundklima_vorort/rheinland-pfalz-saarland/nuerburg_barweiler/_node.html</t>
+  </si>
+  <si>
+    <t>https://www.agrarheute.com/management/betriebsfuehrung/huehnermobil-wirtschaftlich-fiasko-goldesel-580465</t>
+  </si>
+  <si>
+    <t>https://www.agrarheute.com/management/betriebsfuehrung/huehnermobil-wirtschaftlich-fiasko-goldesel-580466</t>
+  </si>
+  <si>
+    <t>https://www.agrarheute.com/management/betriebsfuehrung/huehnermobil-wirtschaftlich-fiasko-goldesel-580467</t>
+  </si>
+  <si>
+    <t>https://www.agrarheute.com/management/betriebsfuehrung/huehnermobil-wirtschaftlich-fiasko-goldesel-580469</t>
+  </si>
+  <si>
+    <t>https://www.agrarheute.com/management/betriebsfuehrung/huehnermobil-wirtschaftlich-fiasko-goldesel-580470</t>
+  </si>
+  <si>
+    <t>https://www.agrarheute.com/management/betriebsfuehrung/huehnermobil-wirtschaftlich-fiasko-goldesel-580472</t>
+  </si>
+  <si>
+    <t>https://www.agrarheute.com/management/betriebsfuehrung/huehnermobil-wirtschaftlich-fiasko-goldesel-580473</t>
+  </si>
+  <si>
+    <t>https://www.agrarheute.com/management/betriebsfuehrung/huehnermobil-wirtschaftlich-fiasko-goldesel-580474</t>
+  </si>
+  <si>
+    <t>https://www.agrarheute.com/management/betriebsfuehrung/huehnermobil-wirtschaftlich-fiasko-goldesel-580475</t>
+  </si>
+  <si>
+    <t>https://llh.hessen.de/pflanze/bewaesserung/in-trockenperioden-richtig-bewaessern-grenzen-der-wasserfass-bewaesserung/</t>
+  </si>
+  <si>
+    <t>http://www.plattform-kvk.de/?p=1020</t>
+  </si>
+  <si>
+    <t>https://www.thuenen.de/media/institute/ak/Allgemein/news/Bodenzustandserhebung_Landwirtschaft_Kurzfassung.pdf</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/epdf/10.1111/j.1365-2486.2011.02408.x</t>
+  </si>
+  <si>
+    <t>Own research</t>
+  </si>
+  <si>
+    <t>own estimate</t>
+  </si>
+  <si>
+    <t>own estimate/experience</t>
+  </si>
+  <si>
+    <t>https://llg.sachsen-anhalt.de/fileadmin/Bibliothek/Politik_und_Verwaltung/MLU/LLFG/Dokumente/04_themen/futterbau_gruenland/18_nach-und-neuansaat-gruenland_flyer.pdf</t>
+  </si>
+  <si>
+    <t>https://www.bmel.de/SharedDocs/FAQs/DE/faq-GAP/FAQ-GAP_List.html</t>
+  </si>
+  <si>
+    <t>https://www.lwk-niedersachsen.de/index.cfm/portal/betriebumwelt/nav/360/article/34324.html</t>
+  </si>
+  <si>
+    <t>own estimates/experience</t>
+  </si>
+  <si>
+    <t>Paul Heimann-Hahues, veterinarian</t>
+  </si>
+  <si>
+    <t>https://www.noen.at/waidhofen/modsiedl-haselnuss-ernteausfall-bewaesserung-letzter-ausweg-raabs-an-der-thaya-haselnuss-haselnussernte-matthias-theurer-ernteausfall-158530378</t>
+  </si>
+  <si>
+    <t>own research</t>
+  </si>
+  <si>
+    <t>https://www.faz.net/aktuell/wirtschaft/klima-energie-und-umwelt/co2-zertifikate-bringen-rekordeinnahmen-strompreis-steigt-17465425.html</t>
+  </si>
+  <si>
+    <t>https://www.co2online.de/service/klima-orakel/beitrag/wie-viele-baeume-braucht-es-um-eine-tonne-co2-zu-binden-10658/</t>
+  </si>
+  <si>
+    <t>https://www.bad-neuenahr-ahrweiler.de/fileadmin/redaktion/stadt/wasserwerk/Preisblatt_Wasser_2016_der_Stadt_BN-AW.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,6 +657,26 @@
     <font>
       <sz val="11"/>
       <color rgb="FF797979"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -625,10 +735,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -641,8 +752,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -957,20 +1072,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B142AC-1DE2-46C2-BBE5-78F1603E233D}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="39" customWidth="1"/>
-    <col min="7" max="7" width="50.109375" customWidth="1"/>
-    <col min="8" max="8" width="62.5546875" customWidth="1"/>
+    <col min="7" max="7" width="50.140625" customWidth="1"/>
+    <col min="8" max="8" width="62.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -996,7 +1111,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
@@ -1015,8 +1130,11 @@
       <c r="F2" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
@@ -1035,8 +1153,11 @@
       <c r="F3" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
@@ -1056,8 +1177,11 @@
         <v>21</v>
       </c>
       <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -1077,8 +1201,11 @@
         <v>22</v>
       </c>
       <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
@@ -1100,8 +1227,11 @@
       <c r="G6" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>35</v>
       </c>
@@ -1121,8 +1251,11 @@
         <v>36</v>
       </c>
       <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
@@ -1142,8 +1275,11 @@
         <v>24</v>
       </c>
       <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>37</v>
       </c>
@@ -1163,8 +1299,11 @@
         <v>38</v>
       </c>
       <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>39</v>
       </c>
@@ -1184,8 +1323,11 @@
         <v>40</v>
       </c>
       <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>41</v>
       </c>
@@ -1205,8 +1347,11 @@
         <v>42</v>
       </c>
       <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1226,8 +1371,11 @@
         <v>28</v>
       </c>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>108</v>
       </c>
@@ -1247,8 +1395,11 @@
         <v>28</v>
       </c>
       <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1268,8 +1419,11 @@
         <v>23</v>
       </c>
       <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1289,8 +1443,11 @@
         <v>30</v>
       </c>
       <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1310,8 +1467,11 @@
         <v>30</v>
       </c>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -1331,8 +1491,11 @@
         <v>44</v>
       </c>
       <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -1352,8 +1515,11 @@
         <v>44</v>
       </c>
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
@@ -1373,8 +1539,11 @@
         <v>47</v>
       </c>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -1394,8 +1563,11 @@
         <v>47</v>
       </c>
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>109</v>
       </c>
@@ -1415,8 +1587,11 @@
         <v>47</v>
       </c>
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>110</v>
       </c>
@@ -1436,8 +1611,11 @@
         <v>47</v>
       </c>
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -1457,8 +1635,11 @@
         <v>50</v>
       </c>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
@@ -1478,8 +1659,11 @@
         <v>50</v>
       </c>
       <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -1499,8 +1683,11 @@
         <v>53</v>
       </c>
       <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1520,8 +1707,11 @@
         <v>55</v>
       </c>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
@@ -1541,8 +1731,11 @@
         <v>55</v>
       </c>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
@@ -1562,8 +1755,11 @@
         <v>58</v>
       </c>
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
@@ -1583,8 +1779,11 @@
         <v>58</v>
       </c>
       <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H29" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>60</v>
       </c>
@@ -1604,8 +1803,11 @@
         <v>61</v>
       </c>
       <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>62</v>
       </c>
@@ -1625,8 +1827,11 @@
         <v>61</v>
       </c>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>63</v>
       </c>
@@ -1646,8 +1851,11 @@
         <v>64</v>
       </c>
       <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H32" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1667,8 +1875,11 @@
         <v>64</v>
       </c>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
@@ -1688,8 +1899,11 @@
         <v>67</v>
       </c>
       <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H34" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -1711,8 +1925,11 @@
       <c r="G35" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H35" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>15</v>
       </c>
@@ -1732,8 +1949,11 @@
         <v>25</v>
       </c>
       <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H36" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>16</v>
       </c>
@@ -1753,8 +1973,11 @@
         <v>26</v>
       </c>
       <c r="G37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H37" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>70</v>
       </c>
@@ -1774,8 +1997,11 @@
         <v>71</v>
       </c>
       <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H38" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>72</v>
       </c>
@@ -1795,8 +2021,11 @@
         <v>73</v>
       </c>
       <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H39" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>74</v>
       </c>
@@ -1816,8 +2045,11 @@
         <v>75</v>
       </c>
       <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H40" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>76</v>
       </c>
@@ -1837,8 +2069,11 @@
         <v>77</v>
       </c>
       <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H41" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>78</v>
       </c>
@@ -1857,8 +2092,11 @@
       <c r="F42" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H42" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>17</v>
       </c>
@@ -1877,8 +2115,11 @@
       <c r="F43" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H43" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>80</v>
       </c>
@@ -1897,8 +2138,11 @@
       <c r="F44" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H44" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>82</v>
       </c>
@@ -1917,8 +2161,11 @@
       <c r="F45" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H45" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>83</v>
       </c>
@@ -1937,8 +2184,11 @@
       <c r="F46" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H46" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>85</v>
       </c>
@@ -1957,8 +2207,11 @@
       <c r="F47" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H47" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>86</v>
       </c>
@@ -1981,7 +2234,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>87</v>
       </c>
@@ -2004,7 +2257,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>104</v>
       </c>
@@ -2027,7 +2280,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>88</v>
       </c>
@@ -2050,7 +2303,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>89</v>
       </c>
@@ -2073,7 +2326,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>91</v>
       </c>
@@ -2096,7 +2349,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>92</v>
       </c>
@@ -2119,7 +2372,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>93</v>
       </c>
@@ -2142,7 +2395,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>112</v>
       </c>
@@ -2161,9 +2414,11 @@
       <c r="F56" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H56" s="3"/>
-    </row>
-    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H56" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>113</v>
       </c>
@@ -2182,9 +2437,11 @@
       <c r="F57" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H57" s="3"/>
-    </row>
-    <row r="58" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H57" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>94</v>
       </c>
@@ -2203,8 +2460,11 @@
       <c r="F58" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H58" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>161</v>
       </c>
@@ -2223,8 +2483,11 @@
       <c r="F59" s="8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H59" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>160</v>
       </c>
@@ -2243,8 +2506,11 @@
       <c r="F60" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H60" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>95</v>
       </c>
@@ -2263,8 +2529,11 @@
       <c r="F61" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H61" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>159</v>
       </c>
@@ -2283,8 +2552,11 @@
       <c r="F62" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H62" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>156</v>
       </c>
@@ -2303,8 +2575,11 @@
       <c r="F63" s="8" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H63" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>158</v>
       </c>
@@ -2323,8 +2598,11 @@
       <c r="F64" s="8" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H64" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>163</v>
       </c>
@@ -2343,8 +2621,11 @@
       <c r="F65" s="8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H65" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>164</v>
       </c>
@@ -2363,8 +2644,11 @@
       <c r="F66" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H66" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>165</v>
       </c>
@@ -2383,8 +2667,11 @@
       <c r="F67" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H67" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>96</v>
       </c>
@@ -2403,8 +2690,11 @@
       <c r="F68" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H68" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>114</v>
       </c>
@@ -2424,7 +2714,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>115</v>
       </c>
@@ -2443,8 +2733,11 @@
       <c r="F70" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H70" s="14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>116</v>
       </c>
@@ -2463,8 +2756,11 @@
       <c r="F71" s="9" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H71" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>117</v>
       </c>
@@ -2483,8 +2779,11 @@
       <c r="F72" s="9" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H72" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>166</v>
       </c>
@@ -2503,8 +2802,11 @@
       <c r="F73" s="9" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H73" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>168</v>
       </c>
@@ -2523,8 +2825,11 @@
       <c r="F74" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H74" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>169</v>
       </c>
@@ -2543,8 +2848,11 @@
       <c r="F75" s="9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H75" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>154</v>
       </c>
@@ -2563,8 +2871,11 @@
       <c r="F76" s="9" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H76" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>122</v>
       </c>
@@ -2583,8 +2894,11 @@
       <c r="F77" s="11" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H77" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>124</v>
       </c>
@@ -2603,8 +2917,11 @@
       <c r="F78" s="11" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H78" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>126</v>
       </c>
@@ -2623,8 +2940,11 @@
       <c r="F79" s="11" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H79" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
         <v>128</v>
       </c>
@@ -2643,8 +2963,11 @@
       <c r="F80" s="11" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H80" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>130</v>
       </c>
@@ -2663,8 +2986,11 @@
       <c r="F81" s="11" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H81" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>132</v>
       </c>
@@ -2683,8 +3009,11 @@
       <c r="F82" s="11" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H82" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>134</v>
       </c>
@@ -2703,8 +3032,11 @@
       <c r="F83" s="11" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H83" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
         <v>136</v>
       </c>
@@ -2723,8 +3055,11 @@
       <c r="F84" s="11" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H84" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>138</v>
       </c>
@@ -2743,8 +3078,11 @@
       <c r="F85" s="11" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H85" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>140</v>
       </c>
@@ -2763,8 +3101,11 @@
       <c r="F86" s="11" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H86" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>142</v>
       </c>
@@ -2783,8 +3124,11 @@
       <c r="F87" s="11" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H87" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>144</v>
       </c>
@@ -2803,8 +3147,11 @@
       <c r="F88" s="11" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H88" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
         <v>146</v>
       </c>
@@ -2823,8 +3170,11 @@
       <c r="F89" s="11" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H89" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
         <v>148</v>
       </c>
@@ -2843,8 +3193,11 @@
       <c r="F90" s="11" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H90" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>150</v>
       </c>
@@ -2863,8 +3216,11 @@
       <c r="F91" s="11" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H91" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
         <v>152</v>
       </c>
@@ -2883,9 +3239,18 @@
       <c r="F92" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="H92" s="11" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H15" r:id="rId1" xr:uid="{65C42029-69F6-4B1E-9F39-666D1A87989B}"/>
+    <hyperlink ref="H61" r:id="rId2" display="https://www.agrarheute.com/management/betriebsfuehrung/huehnermobil-wirtschaftlich-fiasko-goldesel-580468 and own experiences" xr:uid="{FED32897-03FE-4B4A-B7DD-A8DEDCD45D94}"/>
+    <hyperlink ref="H70" r:id="rId3" xr:uid="{16079FEC-043E-41A5-9726-6C1390566928}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>